<commit_message>
Add data for artifical seawater and brackish water, still need to update master table with mineral masses
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaABW_7_11_2017/RaABW Equilibrated Data.xlsx
+++ b/Sorption Experiments/RaABW_7_11_2017/RaABW Equilibrated Data.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\RaABW_7_11_2017\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Equilibrated Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -75,8 +70,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,14 +134,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -193,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,10 +212,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,7 +246,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,16 +421,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,169 +436,169 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21.28722222222223</v>
+        <v>21.23458333333333</v>
       </c>
       <c r="C2">
-        <v>0.37678383333333348</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3763829895833333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>19.984999999999999</v>
+        <v>19.97958333333333</v>
       </c>
       <c r="C3">
-        <v>0.36505933333333329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3651268854166666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>20.198888888888892</v>
+        <v>20.09625</v>
       </c>
       <c r="C4">
-        <v>0.36694648148148151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3662541562500001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>19.633333333333329</v>
+        <v>19.50083333333333</v>
       </c>
       <c r="C5">
-        <v>0.36190777777777777</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3607654166666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>20.231666666666669</v>
+        <v>20.17416666666666</v>
       </c>
       <c r="C6">
-        <v>0.36686755555555561</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3666654791666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>19.812222222222221</v>
+        <v>19.83208333333333</v>
       </c>
       <c r="C7">
-        <v>0.36322407407407398</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3634229270833333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>19.497777777777781</v>
+        <v>19.49041666666667</v>
       </c>
       <c r="C8">
-        <v>0.36070888888888902</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3605727083333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>19.372777777777781</v>
+        <v>19.39791666666667</v>
       </c>
       <c r="C9">
-        <v>0.35968790740740741</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3598313541666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>19.684999999999999</v>
+        <v>19.58791666666666</v>
       </c>
       <c r="C10">
-        <v>0.36220400000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3613970625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>18.666666666666671</v>
+        <v>18.67208333333333</v>
       </c>
       <c r="C11">
-        <v>0.35342222222222219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3533691770833333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>18.98833333333333</v>
+        <v>19.025</v>
       </c>
       <c r="C12">
-        <v>0.35571477777777771</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.356243125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>18.617222222222221</v>
+        <v>18.58416666666667</v>
       </c>
       <c r="C13">
-        <v>0.35186550000000011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3517053541666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>41.276666666666671</v>
+        <v>41.04888888888889</v>
       </c>
       <c r="C14">
-        <v>0.52421366666666669</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5226891851851851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>21.83</v>
+        <v>21.83944444444444</v>
       </c>
       <c r="C15">
-        <v>0.382025</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3821902777777778</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>42.043333333333337</v>
+        <v>41.61666666666667</v>
       </c>
       <c r="C16">
-        <v>0.52974600000000005</v>
+        <v>0.5271444444444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>